<commit_message>
feat: increase merchant diversity in test data (PLAN 1.4)
- Add 20+ unique merchants to SpareBank1 CSV, DNB Excel, and Amex QBO files
- Add merchants that should NOT match patterns (test uncategorized):
  APOTEK 1, BURGER KING, MCDONALDS, PEPPES PIZZA, TANUM, NORLI, SATS,
  ELIXIA, JULA, BILTEMA, CUBUS, KID INTERIØR, IKEA, DRESSMANN, INTERSPORT,
  NILLE, NORMAL, FLYING TIGER, VITA, KICKS, ESSO, CIRCLE K, BUNNPRIS,
  JOKER, ODA.COM, FOODORA, WOLT, JUST EAT, etc.
- Add merchants with similar names for regex specificity tests:
  REMA TORSHOV (missing "1000"), KIWI MINIPRIS, COOP OBS BYGG,
  SPOTIFY FAMILY, NETFLIX PREMIUM, STATOIL EXPRESS, SAS PLUS
- Add merchants with inconsistent casing: Kiwi, kiwi, Starbucks,
  starbucks, Netflix, netflix.com

Each monthly file now has unique, diverse transactions instead of
templated copies, making the test data more realistic for importer testing.
</commit_message>
<xml_diff>
--- a/data/dnb/2025-01.xlsx
+++ b/data/dnb/2025-01.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DNB Mastercard Demo" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45716</v>
+        <v>45688</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -471,7 +471,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45714</v>
+        <v>45687</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -484,7 +484,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45712</v>
+        <v>45685</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -497,132 +497,210 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45710</v>
+        <v>45684</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>REMA 1000 TORSHOV</t>
+          <t>APOTEK 1 SINSEN</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>892.3</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45708</v>
+        <v>45682</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VINMONOPOLET OSLO S</t>
+          <t>REMA 1000 TORSHOV</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>675</v>
+        <v>892.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45706</v>
+        <v>45681</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>STARBUCKS KARL JOHAN</t>
+          <t>BURGER KING KARL JOHAN</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>89</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45703</v>
+        <v>45679</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>GITHUB.COM</t>
+          <t>VINMONOPOLET OSLO S</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>129</v>
+        <v>675</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45700</v>
+        <v>45677</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SAS EUROBONUS</t>
+          <t>STARBUCKS KARL JOHAN</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2890</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45698</v>
+        <v>45675</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MENY BOGSTADVEIEN</t>
+          <t>TANUM BOKHANDEL OSLO</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>567.45</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45696</v>
+        <v>45674</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>POWER STORO</t>
+          <t>GITHUB.COM</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1299</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45693</v>
+        <v>45672</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>COOP EXTRA GRØNLAND</t>
+          <t>SAS EUROBONUS</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>723.9</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45691</v>
+        <v>45671</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Innbetaling</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>15000</v>
+          <t>SATS GYM MAJORSTUEN</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>599</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45689</v>
+        <v>45669</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>MENY BOGSTADVEIEN</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>567.45</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>POWER STORO</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>45665</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MCDONALDS OSLO S</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>45664</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>COOP EXTRA GRØNLAND</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>723.9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>45662</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Innbetaling</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>45660</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>XXL SPORT ALNA</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="F19" t="n">
         <v>1499</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>45659</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PEPPES PIZZA SOLLI</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>